<commit_message>
Fourth commit of project
</commit_message>
<xml_diff>
--- a/backend/templates/RECOVA_LOAN_Import_Template.xlsx
+++ b/backend/templates/RECOVA_LOAN_Import_Template.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,16 +29,16 @@
       <name val="Arial"/>
       <b val="1"/>
       <color rgb="00366092"/>
-      <sz val="14"/>
+      <sz val="16"/>
     </font>
     <font>
       <name val="Arial"/>
-      <i val="1"/>
-      <sz val="10"/>
+      <color rgb="00666666"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
-      <color rgb="00FF0000"/>
+      <color rgb="00CC0000"/>
       <sz val="10"/>
     </font>
     <font>
@@ -46,10 +46,6 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -87,20 +83,18 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -466,68 +460,61 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="27" customWidth="1" min="6" max="6"/>
-    <col width="27" customWidth="1" min="7" max="7"/>
-    <col width="27" customWidth="1" min="8" max="8"/>
-    <col width="17" customWidth="1" min="9" max="9"/>
-    <col width="16" customWidth="1" min="10" max="10"/>
-    <col width="23" customWidth="1" min="11" max="11"/>
-    <col width="19" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="18" customWidth="1" min="14" max="14"/>
-    <col width="27" customWidth="1" min="15" max="15"/>
-    <col width="29" customWidth="1" min="16" max="16"/>
-    <col width="29" customWidth="1" min="17" max="17"/>
-    <col width="29" customWidth="1" min="18" max="18"/>
-    <col width="33" customWidth="1" min="19" max="19"/>
-    <col width="19" customWidth="1" min="20" max="20"/>
-    <col width="21" customWidth="1" min="21" max="21"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
     <col width="12" customWidth="1" min="22" max="22"/>
     <col width="12" customWidth="1" min="23" max="23"/>
     <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="13" customWidth="1" min="25" max="25"/>
-    <col width="15" customWidth="1" min="26" max="26"/>
-    <col width="13" customWidth="1" min="27" max="27"/>
-    <col width="17" customWidth="1" min="28" max="28"/>
-    <col width="24" customWidth="1" min="29" max="29"/>
-    <col width="22" customWidth="1" min="30" max="30"/>
-    <col width="18" customWidth="1" min="31" max="31"/>
-    <col width="22" customWidth="1" min="32" max="32"/>
-    <col width="17" customWidth="1" min="33" max="33"/>
-    <col width="30" customWidth="1" min="34" max="34"/>
-    <col width="30" customWidth="1" min="35" max="35"/>
-    <col width="18" customWidth="1" min="36" max="36"/>
-    <col width="24" customWidth="1" min="37" max="37"/>
-    <col width="17" customWidth="1" min="38" max="38"/>
-    <col width="30" customWidth="1" min="39" max="39"/>
-    <col width="30" customWidth="1" min="40" max="40"/>
-    <col width="14" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="25" max="25"/>
+    <col width="12" customWidth="1" min="26" max="26"/>
+    <col width="12" customWidth="1" min="27" max="27"/>
+    <col width="12" customWidth="1" min="28" max="28"/>
+    <col width="12" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="12" customWidth="1" min="32" max="32"/>
+    <col width="12" customWidth="1" min="33" max="33"/>
+    <col width="12" customWidth="1" min="34" max="34"/>
+    <col width="12" customWidth="1" min="35" max="35"/>
+    <col width="12" customWidth="1" min="36" max="36"/>
+    <col width="12" customWidth="1" min="37" max="37"/>
+    <col width="12" customWidth="1" min="38" max="38"/>
+    <col width="12" customWidth="1" min="39" max="39"/>
+    <col width="12" customWidth="1" min="40" max="40"/>
+    <col width="12" customWidth="1" min="41" max="41"/>
     <col width="12" customWidth="1" min="42" max="42"/>
-    <col width="13" customWidth="1" min="43" max="43"/>
-    <col width="36" customWidth="1" min="44" max="44"/>
-    <col width="15" customWidth="1" min="45" max="45"/>
-    <col width="17" customWidth="1" min="46" max="46"/>
-    <col width="27" customWidth="1" min="47" max="47"/>
-    <col width="30" customWidth="1" min="48" max="48"/>
-    <col width="20" customWidth="1" min="49" max="49"/>
-    <col width="26" customWidth="1" min="50" max="50"/>
-    <col width="23" customWidth="1" min="51" max="51"/>
-    <col width="34" customWidth="1" min="52" max="52"/>
-    <col width="16" customWidth="1" min="53" max="53"/>
-    <col width="26" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -540,36 +527,36 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Loan defaulter accounts template with bank information and all customer/loan-specific fields</t>
+          <t>Import Template for Loan Operations</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Instructions: Fill in the data starting from row 6. Do not modify the headers in row 5.</t>
+          <t>Important: client_code must match the selected client. Fill all required fields marked with *</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Bank Name</t>
+          <t>Client Code *</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Operation Name</t>
+          <t>Contract Number *</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>Client Name</t>
+          <t>Client Name *</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>Nic</t>
+          <t>Nic *</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -594,718 +581,579 @@
       </c>
       <c r="I5" s="4" t="inlineStr">
         <is>
-          <t>Contract Number</t>
+          <t>Granted Amount</t>
         </is>
       </c>
       <c r="J5" s="4" t="inlineStr">
         <is>
-          <t>Granted Amount</t>
+          <t>Facility Granted Date</t>
         </is>
       </c>
       <c r="K5" s="4" t="inlineStr">
         <is>
-          <t>Facility Granted Date</t>
+          <t>Facility End Date</t>
         </is>
       </c>
       <c r="L5" s="4" t="inlineStr">
         <is>
-          <t>Facility End Date</t>
+          <t>Monthly Rental Payment With Vat</t>
         </is>
       </c>
       <c r="M5" s="4" t="inlineStr">
         <is>
+          <t>Last Payment Date</t>
+        </is>
+      </c>
+      <c r="N5" s="4" t="inlineStr">
+        <is>
+          <t>Last Payment Amount</t>
+        </is>
+      </c>
+      <c r="O5" s="4" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+      <c r="P5" s="4" t="inlineStr">
+        <is>
           <t>Designation</t>
         </is>
       </c>
-      <c r="N5" s="4" t="inlineStr">
+      <c r="Q5" s="4" t="inlineStr">
         <is>
           <t>Work Place Name</t>
         </is>
       </c>
-      <c r="O5" s="4" t="inlineStr">
+      <c r="R5" s="4" t="inlineStr">
         <is>
           <t>Work Place Address</t>
         </is>
       </c>
-      <c r="P5" s="4" t="inlineStr">
+      <c r="S5" s="4" t="inlineStr">
         <is>
           <t>Work Place Contact Number 1</t>
         </is>
       </c>
-      <c r="Q5" s="4" t="inlineStr">
+      <c r="T5" s="4" t="inlineStr">
         <is>
           <t>Work Place Contact Number 2</t>
         </is>
       </c>
-      <c r="R5" s="4" t="inlineStr">
+      <c r="U5" s="4" t="inlineStr">
         <is>
           <t>Work Place Contact Number 3</t>
         </is>
       </c>
-      <c r="S5" s="4" t="inlineStr">
-        <is>
-          <t>Monthly Rental Payment With Vat</t>
-        </is>
-      </c>
-      <c r="T5" s="4" t="inlineStr">
-        <is>
-          <t>Last Payment Date</t>
-        </is>
-      </c>
-      <c r="U5" s="4" t="inlineStr">
-        <is>
-          <t>Last Payment Amount</t>
-        </is>
-      </c>
       <c r="V5" s="4" t="inlineStr">
         <is>
-          <t>Due Date</t>
+          <t>Guarantor 1 Name</t>
         </is>
       </c>
       <c r="W5" s="4" t="inlineStr">
         <is>
+          <t>Guarantor 1 Address</t>
+        </is>
+      </c>
+      <c r="X5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 1 Nic</t>
+        </is>
+      </c>
+      <c r="Y5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 1 Contact Number 1</t>
+        </is>
+      </c>
+      <c r="Z5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 1 Contact Number 2</t>
+        </is>
+      </c>
+      <c r="AA5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 2 Name</t>
+        </is>
+      </c>
+      <c r="AB5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 2 Address</t>
+        </is>
+      </c>
+      <c r="AC5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 2 Nic</t>
+        </is>
+      </c>
+      <c r="AD5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 2 Contact Number 1</t>
+        </is>
+      </c>
+      <c r="AE5" s="4" t="inlineStr">
+        <is>
+          <t>Guarantor 2 Contact Number 2</t>
+        </is>
+      </c>
+      <c r="AF5" s="4" t="inlineStr">
+        <is>
           <t>Zone</t>
         </is>
       </c>
-      <c r="X5" s="4" t="inlineStr">
+      <c r="AG5" s="4" t="inlineStr">
         <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="Y5" s="4" t="inlineStr">
+      <c r="AH5" s="4" t="inlineStr">
         <is>
           <t>Branch Name</t>
         </is>
       </c>
-      <c r="Z5" s="4" t="inlineStr">
+      <c r="AI5" s="4" t="inlineStr">
         <is>
           <t>District Name</t>
         </is>
       </c>
-      <c r="AA5" s="4" t="inlineStr">
+      <c r="AJ5" s="4" t="inlineStr">
         <is>
           <t>Postal Town</t>
         </is>
       </c>
-      <c r="AB5" s="4" t="inlineStr">
+      <c r="AK5" s="4" t="inlineStr">
         <is>
           <t>Days In Arrears</t>
         </is>
       </c>
-      <c r="AC5" s="4" t="inlineStr">
+      <c r="AL5" s="4" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
-      <c r="AD5" s="4" t="inlineStr">
+      <c r="AM5" s="4" t="inlineStr">
         <is>
           <t>Payment Assumption</t>
         </is>
       </c>
-      <c r="AE5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 1 Name</t>
-        </is>
-      </c>
-      <c r="AF5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 1 Address</t>
-        </is>
-      </c>
-      <c r="AG5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 1 Nic</t>
-        </is>
-      </c>
-      <c r="AH5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 1 Contact Number 1</t>
-        </is>
-      </c>
-      <c r="AI5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 1 Contact Number 2</t>
-        </is>
-      </c>
-      <c r="AJ5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 2 Name</t>
-        </is>
-      </c>
-      <c r="AK5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 2 Address</t>
-        </is>
-      </c>
-      <c r="AL5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 2 Nic</t>
-        </is>
-      </c>
-      <c r="AM5" s="4" t="inlineStr">
-        <is>
-          <t>Guarantor 2 Contact Number 1</t>
-        </is>
-      </c>
       <c r="AN5" s="4" t="inlineStr">
         <is>
-          <t>Guarantor 2 Contact Number 2</t>
+          <t>Loan Type</t>
         </is>
       </c>
       <c r="AO5" s="4" t="inlineStr">
         <is>
-          <t>Segment</t>
+          <t>Loan Amount</t>
         </is>
       </c>
       <c r="AP5" s="4" t="inlineStr">
         <is>
-          <t>Loan Type</t>
+          <t>Installment Amount</t>
         </is>
       </c>
       <c r="AQ5" s="4" t="inlineStr">
         <is>
-          <t>Loan Status</t>
+          <t>Outstanding Balance</t>
         </is>
       </c>
       <c r="AR5" s="4" t="inlineStr">
         <is>
-          <t>Loan Description</t>
+          <t>Interest Rate</t>
         </is>
       </c>
       <c r="AS5" s="4" t="inlineStr">
         <is>
-          <t>Clear Balance</t>
+          <t>Loan Term Months</t>
         </is>
       </c>
       <c r="AT5" s="4" t="inlineStr">
         <is>
-          <t>Capital Balance</t>
-        </is>
-      </c>
-      <c r="AU5" s="4" t="inlineStr">
-        <is>
-          <t>Interest Over Due Balance</t>
-        </is>
-      </c>
-      <c r="AV5" s="4" t="inlineStr">
-        <is>
-          <t>Capital With Interest Amount</t>
-        </is>
-      </c>
-      <c r="AW5" s="4" t="inlineStr">
-        <is>
-          <t>Installment Amount</t>
-        </is>
-      </c>
-      <c r="AX5" s="4" t="inlineStr">
-        <is>
-          <t>Arrears Settlement Offer</t>
-        </is>
-      </c>
-      <c r="AY5" s="4" t="inlineStr">
-        <is>
-          <t>Full Settlement Offer</t>
-        </is>
-      </c>
-      <c r="AZ5" s="4" t="inlineStr">
-        <is>
-          <t>Security Description</t>
-        </is>
-      </c>
-      <c r="BA5" s="4" t="inlineStr">
-        <is>
-          <t>Security Value</t>
-        </is>
-      </c>
-      <c r="BB5" s="4" t="inlineStr">
-        <is>
-          <t>Operative Account Number</t>
+          <t>Remaining Installments</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Sampath Bank</t>
+          <t>SAMPBANK</t>
         </is>
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Loans</t>
+          <t>LN001234567</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>234567890V</t>
+          <t>345678901V</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>789 Oak Road, Kandy</t>
+          <t>789 Third St, Galle</t>
         </is>
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>0712345678</t>
+          <t>0771111111</t>
         </is>
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>0812345679</t>
+          <t>0912222222</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr"/>
-      <c r="I6" s="5" t="inlineStr">
-        <is>
-          <t>LN987654321</t>
-        </is>
-      </c>
-      <c r="J6" s="5" t="n">
+      <c r="I6" s="5" t="n">
         <v>1000000</v>
       </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>2022-01-10</t>
+        </is>
+      </c>
       <c r="K6" s="5" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
-        </is>
-      </c>
-      <c r="L6" s="5" t="inlineStr">
-        <is>
-          <t>2027-05-10</t>
-        </is>
+          <t>2027-01-10</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>25000</v>
       </c>
       <c r="M6" s="5" t="inlineStr">
         <is>
-          <t>Engineer</t>
-        </is>
-      </c>
-      <c r="N6" s="5" t="inlineStr">
-        <is>
-          <t>XYZ Corporation</t>
-        </is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>22000</v>
       </c>
       <c r="O6" s="5" t="inlineStr">
         <is>
-          <t>123 Tech Park, Kandy</t>
+          <t>2025-08-10</t>
         </is>
       </c>
       <c r="P6" s="5" t="inlineStr">
         <is>
-          <t>0812233445</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="Q6" s="5" t="inlineStr">
         <is>
-          <t>0812233446</t>
-        </is>
-      </c>
-      <c r="R6" s="5" t="inlineStr"/>
-      <c r="S6" s="5" t="n">
-        <v>15000</v>
+          <t>DEF Industries</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>111 Industrial Rd, Galle</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr">
+        <is>
+          <t>0912345678</t>
+        </is>
       </c>
       <c r="T6" s="5" t="inlineStr">
         <is>
-          <t>2025-07-10</t>
-        </is>
-      </c>
-      <c r="U6" s="5" t="n">
-        <v>12000</v>
-      </c>
+          <t>0919876543</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr"/>
       <c r="V6" s="5" t="inlineStr">
         <is>
-          <t>2025-08-10</t>
+          <t>Mike Johnson</t>
         </is>
       </c>
       <c r="W6" s="5" t="inlineStr">
         <is>
-          <t>Kandy</t>
+          <t>222 Brother St, Matara</t>
         </is>
       </c>
       <c r="X6" s="5" t="inlineStr">
         <is>
-          <t>Central</t>
+          <t>567890123V</t>
         </is>
       </c>
       <c r="Y6" s="5" t="inlineStr">
         <is>
-          <t>Kandy Main</t>
+          <t>0774444444</t>
         </is>
       </c>
       <c r="Z6" s="5" t="inlineStr">
         <is>
-          <t>Kandy</t>
+          <t>0913333333</t>
         </is>
       </c>
       <c r="AA6" s="5" t="inlineStr">
         <is>
-          <t>Kandy 20000</t>
-        </is>
-      </c>
-      <c r="AB6" s="5" t="n">
-        <v>30</v>
+          <t>Sarah Wilson</t>
+        </is>
+      </c>
+      <c r="AB6" s="5" t="inlineStr">
+        <is>
+          <t>333 Sister St, Hikkaduwa</t>
+        </is>
       </c>
       <c r="AC6" s="5" t="inlineStr">
         <is>
-          <t>Property loan</t>
+          <t>678901234V</t>
         </is>
       </c>
       <c r="AD6" s="5" t="inlineStr">
         <is>
+          <t>0775555555</t>
+        </is>
+      </c>
+      <c r="AE6" s="5" t="inlineStr"/>
+      <c r="AF6" s="5" t="inlineStr">
+        <is>
+          <t>Southern</t>
+        </is>
+      </c>
+      <c r="AG6" s="5" t="inlineStr">
+        <is>
+          <t>Galle</t>
+        </is>
+      </c>
+      <c r="AH6" s="5" t="inlineStr">
+        <is>
+          <t>Galle Fort</t>
+        </is>
+      </c>
+      <c r="AI6" s="5" t="inlineStr">
+        <is>
+          <t>Galle</t>
+        </is>
+      </c>
+      <c r="AJ6" s="5" t="inlineStr">
+        <is>
+          <t>Galle</t>
+        </is>
+      </c>
+      <c r="AK6" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="AL6" s="5" t="inlineStr">
+        <is>
+          <t>Housing loan customer</t>
+        </is>
+      </c>
+      <c r="AM6" s="5" t="inlineStr">
+        <is>
           <t>Monthly installments</t>
         </is>
       </c>
-      <c r="AE6" s="5" t="inlineStr">
-        <is>
-          <t>Bob Smith</t>
-        </is>
-      </c>
-      <c r="AF6" s="5" t="inlineStr">
-        <is>
-          <t>456 Hill Road, Kandy</t>
-        </is>
-      </c>
-      <c r="AG6" s="5" t="inlineStr">
-        <is>
-          <t>345678901V</t>
-        </is>
-      </c>
-      <c r="AH6" s="5" t="inlineStr">
-        <is>
-          <t>0713456789</t>
-        </is>
-      </c>
-      <c r="AI6" s="5" t="inlineStr">
-        <is>
-          <t>0813456789</t>
-        </is>
-      </c>
-      <c r="AJ6" s="5" t="inlineStr">
-        <is>
-          <t>Carol Johnson</t>
-        </is>
-      </c>
-      <c r="AK6" s="5" t="inlineStr">
-        <is>
-          <t>789 Valley Road, Kandy</t>
-        </is>
-      </c>
-      <c r="AL6" s="5" t="inlineStr">
-        <is>
-          <t>567890123V</t>
-        </is>
-      </c>
-      <c r="AM6" s="5" t="inlineStr">
-        <is>
-          <t>0714567890</t>
-        </is>
-      </c>
       <c r="AN6" s="5" t="inlineStr">
         <is>
-          <t>0814567890</t>
-        </is>
-      </c>
-      <c r="AO6" s="5" t="inlineStr">
-        <is>
-          <t>RETAIL</t>
-        </is>
-      </c>
-      <c r="AP6" s="5" t="inlineStr">
-        <is>
-          <t>PERSONAL</t>
-        </is>
-      </c>
-      <c r="AQ6" s="5" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
-      <c r="AR6" s="5" t="inlineStr">
-        <is>
-          <t>Personal loan for house renovation</t>
-        </is>
+          <t>Housing Loan</t>
+        </is>
+      </c>
+      <c r="AO6" s="5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="AP6" s="5" t="n">
+        <v>25000</v>
+      </c>
+      <c r="AQ6" s="5" t="n">
+        <v>750000</v>
+      </c>
+      <c r="AR6" s="5" t="n">
+        <v>8.5</v>
       </c>
       <c r="AS6" s="5" t="n">
-        <v>50000</v>
+        <v>60</v>
       </c>
       <c r="AT6" s="5" t="n">
-        <v>750000</v>
-      </c>
-      <c r="AU6" s="5" t="n">
-        <v>50000</v>
-      </c>
-      <c r="AV6" s="5" t="n">
-        <v>800000</v>
-      </c>
-      <c r="AW6" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="AX6" s="5" t="n">
-        <v>600000</v>
-      </c>
-      <c r="AY6" s="5" t="n">
-        <v>750000</v>
-      </c>
-      <c r="AZ6" s="5" t="inlineStr">
-        <is>
-          <t>Property at Kandy valued at 1.5M</t>
-        </is>
-      </c>
-      <c r="BA6" s="5" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="BB6" s="5" t="inlineStr">
-        <is>
-          <t>OP123456789</t>
-        </is>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>Sampath Bank</t>
+          <t>SEYLAN</t>
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Loans</t>
+          <t>LN987654321</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Bob Wilson</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>345678901V</t>
+          <t>456789012V</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>456 Castle Road, Galle</t>
+          <t>321 Fourth St, Matara</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>0913456789</t>
+          <t>0772222222</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
-          <t>0713456780</t>
-        </is>
-      </c>
-      <c r="H7" s="5" t="inlineStr"/>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>LN876543210</t>
-        </is>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>1500000</v>
+          <t>0412345678</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>0778888888</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>2500000</v>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>2023-06-15</t>
+        </is>
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>2021-08-15</t>
-        </is>
-      </c>
-      <c r="L7" s="5" t="inlineStr">
-        <is>
-          <t>2026-08-15</t>
-        </is>
+          <t>2028-06-15</t>
+        </is>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>45000</v>
       </c>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>Doctor</t>
-        </is>
-      </c>
-      <c r="N7" s="5" t="inlineStr">
-        <is>
-          <t>Private Practice</t>
-        </is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>40000</v>
       </c>
       <c r="O7" s="5" t="inlineStr">
         <is>
-          <t>789 Medical Center, Galle</t>
+          <t>2025-08-15</t>
         </is>
       </c>
       <c r="P7" s="5" t="inlineStr">
         <is>
-          <t>0913334455</t>
-        </is>
-      </c>
-      <c r="Q7" s="5" t="inlineStr"/>
-      <c r="R7" s="5" t="inlineStr"/>
-      <c r="S7" s="5" t="n">
-        <v>25000</v>
-      </c>
-      <c r="T7" s="5" t="inlineStr">
-        <is>
-          <t>2025-07-05</t>
-        </is>
-      </c>
-      <c r="U7" s="5" t="n">
-        <v>22000</v>
-      </c>
+          <t>Manager</t>
+        </is>
+      </c>
+      <c r="Q7" s="5" t="inlineStr">
+        <is>
+          <t>GHI Trading</t>
+        </is>
+      </c>
+      <c r="R7" s="5" t="inlineStr">
+        <is>
+          <t>444 Trade St, Matara</t>
+        </is>
+      </c>
+      <c r="S7" s="5" t="inlineStr">
+        <is>
+          <t>0412223344</t>
+        </is>
+      </c>
+      <c r="T7" s="5" t="inlineStr"/>
+      <c r="U7" s="5" t="inlineStr"/>
       <c r="V7" s="5" t="inlineStr">
         <is>
-          <t>2025-08-05</t>
+          <t>Lisa Wilson</t>
         </is>
       </c>
       <c r="W7" s="5" t="inlineStr">
         <is>
-          <t>Galle</t>
+          <t>555 Wife St, Weligama</t>
         </is>
       </c>
       <c r="X7" s="5" t="inlineStr">
         <is>
+          <t>789012345V</t>
+        </is>
+      </c>
+      <c r="Y7" s="5" t="inlineStr">
+        <is>
+          <t>0776666666</t>
+        </is>
+      </c>
+      <c r="Z7" s="5" t="inlineStr"/>
+      <c r="AA7" s="5" t="inlineStr"/>
+      <c r="AB7" s="5" t="inlineStr"/>
+      <c r="AC7" s="5" t="inlineStr"/>
+      <c r="AD7" s="5" t="inlineStr"/>
+      <c r="AE7" s="5" t="inlineStr"/>
+      <c r="AF7" s="5" t="inlineStr"/>
+      <c r="AG7" s="5" t="inlineStr">
+        <is>
           <t>Southern</t>
         </is>
       </c>
-      <c r="Y7" s="5" t="inlineStr">
-        <is>
-          <t>Galle Main</t>
-        </is>
-      </c>
-      <c r="Z7" s="5" t="inlineStr">
-        <is>
-          <t>Galle</t>
-        </is>
-      </c>
-      <c r="AA7" s="5" t="inlineStr">
-        <is>
-          <t>Galle 80000</t>
-        </is>
-      </c>
-      <c r="AB7" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AC7" s="5" t="inlineStr">
-        <is>
-          <t>Medical equipment loan</t>
-        </is>
-      </c>
-      <c r="AD7" s="5" t="inlineStr">
+      <c r="AH7" s="5" t="inlineStr">
+        <is>
+          <t>Matara</t>
+        </is>
+      </c>
+      <c r="AI7" s="5" t="inlineStr">
+        <is>
+          <t>Matara Main</t>
+        </is>
+      </c>
+      <c r="AJ7" s="5" t="inlineStr">
+        <is>
+          <t>Matara</t>
+        </is>
+      </c>
+      <c r="AK7" s="5" t="inlineStr">
+        <is>
+          <t>Matara</t>
+        </is>
+      </c>
+      <c r="AL7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="AM7" s="5" t="inlineStr">
+        <is>
+          <t>Business loan</t>
+        </is>
+      </c>
+      <c r="AN7" s="5" t="inlineStr">
         <is>
           <t>Regular payments</t>
         </is>
       </c>
-      <c r="AE7" s="5" t="inlineStr">
-        <is>
-          <t>Sarah Brown</t>
-        </is>
-      </c>
-      <c r="AF7" s="5" t="inlineStr">
-        <is>
-          <t>Same address</t>
-        </is>
-      </c>
-      <c r="AG7" s="5" t="inlineStr">
-        <is>
-          <t>456789012V</t>
-        </is>
-      </c>
-      <c r="AH7" s="5" t="inlineStr">
-        <is>
-          <t>0914567890</t>
-        </is>
-      </c>
-      <c r="AI7" s="5" t="inlineStr"/>
-      <c r="AJ7" s="5" t="inlineStr">
-        <is>
-          <t>Michael Wilson</t>
-        </is>
-      </c>
-      <c r="AK7" s="5" t="inlineStr">
-        <is>
-          <t>321 Beach Road, Galle</t>
-        </is>
-      </c>
-      <c r="AL7" s="5" t="inlineStr">
-        <is>
-          <t>678901234V</t>
-        </is>
-      </c>
-      <c r="AM7" s="5" t="inlineStr">
-        <is>
-          <t>0915678901</t>
-        </is>
-      </c>
-      <c r="AN7" s="5" t="inlineStr"/>
       <c r="AO7" s="5" t="inlineStr">
         <is>
-          <t>PROFESSIONAL</t>
-        </is>
-      </c>
-      <c r="AP7" s="5" t="inlineStr">
-        <is>
-          <t>COMMERCIAL</t>
-        </is>
-      </c>
-      <c r="AQ7" s="5" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
-      <c r="AR7" s="5" t="inlineStr">
-        <is>
-          <t>Medical equipment financing</t>
-        </is>
+          <t>Business Loan</t>
+        </is>
+      </c>
+      <c r="AP7" s="5" t="n">
+        <v>2500000</v>
+      </c>
+      <c r="AQ7" s="5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="AR7" s="5" t="n">
+        <v>1850000</v>
       </c>
       <c r="AS7" s="5" t="n">
-        <v>100000</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AT7" s="5" t="n">
-        <v>1200000</v>
-      </c>
-      <c r="AU7" s="5" t="n">
-        <v>75000</v>
-      </c>
-      <c r="AV7" s="5" t="n">
-        <v>1275000</v>
-      </c>
-      <c r="AW7" s="5" t="n">
-        <v>25000</v>
-      </c>
-      <c r="AX7" s="5" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="AY7" s="5" t="n">
-        <v>1200000</v>
-      </c>
-      <c r="AZ7" s="5" t="inlineStr">
-        <is>
-          <t>Medical equipment valued at 2M</t>
-        </is>
-      </c>
-      <c r="BA7" s="5" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="BB7" s="5" t="inlineStr">
-        <is>
-          <t>OP987654321</t>
-        </is>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation sqref="D6:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid NIC Format" error="NIC must be 10-12 characters (e.g., 123456789V or 123456789012)" type="textLength" operator="between">
-      <formula1>10</formula1>
-      <formula2>12</formula2>
-    </dataValidation>
-    <dataValidation sqref="AP6:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Invalid Loan Type" error="Please select a valid loan type" type="list">
-      <formula1>"MORTGAGED,PERSONAL,EDUCATIONAL,VEHICLE,OVERDUE,COMMERCIAL"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>